<commit_message>
add statistical data desribe after encoding from string to numerical
</commit_message>
<xml_diff>
--- a/results/data_info.xlsx
+++ b/results/data_info.xlsx
@@ -1024,7 +1024,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:X9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1083,6 +1083,71 @@
           <t>Performance in online</t>
         </is>
       </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Gender</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Home Location</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Level of Education</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Device type used to attend classes</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Economic status</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Are you involved in any sports?</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Do elderly people monitor you?</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>Interested in Gaming?</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>Have separate room for studying?</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>Engaged in group studies?</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>Average marks scored before pandemic in traditional classroom</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>Interested in?</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>Your level of satisfaction in Online Education</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -1120,6 +1185,45 @@
       <c r="K2" t="n">
         <v>1033</v>
       </c>
+      <c r="L2" t="n">
+        <v>1033</v>
+      </c>
+      <c r="M2" t="n">
+        <v>1033</v>
+      </c>
+      <c r="N2" t="n">
+        <v>1033</v>
+      </c>
+      <c r="O2" t="n">
+        <v>1033</v>
+      </c>
+      <c r="P2" t="n">
+        <v>1033</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>1033</v>
+      </c>
+      <c r="R2" t="n">
+        <v>1033</v>
+      </c>
+      <c r="S2" t="n">
+        <v>1033</v>
+      </c>
+      <c r="T2" t="n">
+        <v>1033</v>
+      </c>
+      <c r="U2" t="n">
+        <v>1033</v>
+      </c>
+      <c r="V2" t="n">
+        <v>1033</v>
+      </c>
+      <c r="W2" t="n">
+        <v>1033</v>
+      </c>
+      <c r="X2" t="n">
+        <v>1033</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -1157,6 +1261,45 @@
       <c r="K3" t="n">
         <v>6.696030977734753</v>
       </c>
+      <c r="L3" t="n">
+        <v>0.5943852855759922</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0.6573088092933205</v>
+      </c>
+      <c r="N3" t="n">
+        <v>1.040658276863504</v>
+      </c>
+      <c r="O3" t="n">
+        <v>0.7028073572120038</v>
+      </c>
+      <c r="P3" t="n">
+        <v>0.9816069699903195</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>0.3581800580832527</v>
+      </c>
+      <c r="R3" t="n">
+        <v>0.5275895450145208</v>
+      </c>
+      <c r="S3" t="n">
+        <v>0.542110358180058</v>
+      </c>
+      <c r="T3" t="n">
+        <v>0.5885769603097774</v>
+      </c>
+      <c r="U3" t="n">
+        <v>0.4036786060019361</v>
+      </c>
+      <c r="V3" t="n">
+        <v>8.235237173281703</v>
+      </c>
+      <c r="W3" t="n">
+        <v>1.096805421103582</v>
+      </c>
+      <c r="X3" t="n">
+        <v>1.009680542110358</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -1194,6 +1337,45 @@
       <c r="K4" t="n">
         <v>1.920047673576594</v>
       </c>
+      <c r="L4" t="n">
+        <v>0.4912484438466198</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0.474839138908102</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0.4556836932206187</v>
+      </c>
+      <c r="O4" t="n">
+        <v>0.5112701339490697</v>
+      </c>
+      <c r="P4" t="n">
+        <v>0.2760647681802985</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>0.4796976786440687</v>
+      </c>
+      <c r="R4" t="n">
+        <v>0.4994800571469162</v>
+      </c>
+      <c r="S4" t="n">
+        <v>0.4984648909393652</v>
+      </c>
+      <c r="T4" t="n">
+        <v>0.4923299377139618</v>
+      </c>
+      <c r="U4" t="n">
+        <v>0.4908721289637493</v>
+      </c>
+      <c r="V4" t="n">
+        <v>1.418263133821204</v>
+      </c>
+      <c r="W4" t="n">
+        <v>0.7524633048108473</v>
+      </c>
+      <c r="X4" t="n">
+        <v>0.6903987125885244</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -1231,6 +1413,45 @@
       <c r="K5" t="n">
         <v>2</v>
       </c>
+      <c r="L5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O5" t="n">
+        <v>0</v>
+      </c>
+      <c r="P5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>0</v>
+      </c>
+      <c r="R5" t="n">
+        <v>0</v>
+      </c>
+      <c r="S5" t="n">
+        <v>0</v>
+      </c>
+      <c r="T5" t="n">
+        <v>0</v>
+      </c>
+      <c r="U5" t="n">
+        <v>0</v>
+      </c>
+      <c r="V5" t="n">
+        <v>1</v>
+      </c>
+      <c r="W5" t="n">
+        <v>0</v>
+      </c>
+      <c r="X5" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -1268,6 +1489,45 @@
       <c r="K6" t="n">
         <v>6</v>
       </c>
+      <c r="L6" t="n">
+        <v>0</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N6" t="n">
+        <v>1</v>
+      </c>
+      <c r="O6" t="n">
+        <v>0</v>
+      </c>
+      <c r="P6" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>0</v>
+      </c>
+      <c r="R6" t="n">
+        <v>0</v>
+      </c>
+      <c r="S6" t="n">
+        <v>0</v>
+      </c>
+      <c r="T6" t="n">
+        <v>0</v>
+      </c>
+      <c r="U6" t="n">
+        <v>0</v>
+      </c>
+      <c r="V6" t="n">
+        <v>8</v>
+      </c>
+      <c r="W6" t="n">
+        <v>1</v>
+      </c>
+      <c r="X6" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -1305,6 +1565,45 @@
       <c r="K7" t="n">
         <v>7</v>
       </c>
+      <c r="L7" t="n">
+        <v>1</v>
+      </c>
+      <c r="M7" t="n">
+        <v>1</v>
+      </c>
+      <c r="N7" t="n">
+        <v>1</v>
+      </c>
+      <c r="O7" t="n">
+        <v>1</v>
+      </c>
+      <c r="P7" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>0</v>
+      </c>
+      <c r="R7" t="n">
+        <v>1</v>
+      </c>
+      <c r="S7" t="n">
+        <v>1</v>
+      </c>
+      <c r="T7" t="n">
+        <v>1</v>
+      </c>
+      <c r="U7" t="n">
+        <v>0</v>
+      </c>
+      <c r="V7" t="n">
+        <v>8</v>
+      </c>
+      <c r="W7" t="n">
+        <v>1</v>
+      </c>
+      <c r="X7" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -1342,6 +1641,45 @@
       <c r="K8" t="n">
         <v>8</v>
       </c>
+      <c r="L8" t="n">
+        <v>1</v>
+      </c>
+      <c r="M8" t="n">
+        <v>1</v>
+      </c>
+      <c r="N8" t="n">
+        <v>1</v>
+      </c>
+      <c r="O8" t="n">
+        <v>1</v>
+      </c>
+      <c r="P8" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>1</v>
+      </c>
+      <c r="R8" t="n">
+        <v>1</v>
+      </c>
+      <c r="S8" t="n">
+        <v>1</v>
+      </c>
+      <c r="T8" t="n">
+        <v>1</v>
+      </c>
+      <c r="U8" t="n">
+        <v>1</v>
+      </c>
+      <c r="V8" t="n">
+        <v>9</v>
+      </c>
+      <c r="W8" t="n">
+        <v>2</v>
+      </c>
+      <c r="X8" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
@@ -1378,6 +1716,45 @@
       </c>
       <c r="K9" t="n">
         <v>10</v>
+      </c>
+      <c r="L9" t="n">
+        <v>1</v>
+      </c>
+      <c r="M9" t="n">
+        <v>1</v>
+      </c>
+      <c r="N9" t="n">
+        <v>2</v>
+      </c>
+      <c r="O9" t="n">
+        <v>2</v>
+      </c>
+      <c r="P9" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>1</v>
+      </c>
+      <c r="R9" t="n">
+        <v>1</v>
+      </c>
+      <c r="S9" t="n">
+        <v>1</v>
+      </c>
+      <c r="T9" t="n">
+        <v>1</v>
+      </c>
+      <c r="U9" t="n">
+        <v>1</v>
+      </c>
+      <c r="V9" t="n">
+        <v>10</v>
+      </c>
+      <c r="W9" t="n">
+        <v>2</v>
+      </c>
+      <c r="X9" t="n">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add [DescribeAfterEncoding] sheet in the results
</commit_message>
<xml_diff>
--- a/results/data_info.xlsx
+++ b/results/data_info.xlsx
@@ -9,6 +9,7 @@
   <sheets>
     <sheet name="Info" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Describe" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="DescribeAfterEncoding" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1024,6 +1025,373 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:K9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Age(Years)</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Number of Subjects</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Family size</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Internet facility in your locality</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Study time (Hours)</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Sleep time (Hours)</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Time spent on social media (Hours)</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Your interaction in online mode</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Clearing doubts with faculties in online mode</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Performance in online</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>count</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>1033</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1033</v>
+      </c>
+      <c r="D2" t="n">
+        <v>1033</v>
+      </c>
+      <c r="E2" t="n">
+        <v>1033</v>
+      </c>
+      <c r="F2" t="n">
+        <v>1033</v>
+      </c>
+      <c r="G2" t="n">
+        <v>1033</v>
+      </c>
+      <c r="H2" t="n">
+        <v>1033</v>
+      </c>
+      <c r="I2" t="n">
+        <v>1033</v>
+      </c>
+      <c r="J2" t="n">
+        <v>1033</v>
+      </c>
+      <c r="K2" t="n">
+        <v>1033</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>mean</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>19.79864472410455</v>
+      </c>
+      <c r="C3" t="n">
+        <v>7.034849951597289</v>
+      </c>
+      <c r="D3" t="n">
+        <v>4.413359148112295</v>
+      </c>
+      <c r="E3" t="n">
+        <v>3.586640851887706</v>
+      </c>
+      <c r="F3" t="n">
+        <v>4.325266214908035</v>
+      </c>
+      <c r="G3" t="n">
+        <v>6.947725072604066</v>
+      </c>
+      <c r="H3" t="n">
+        <v>2.636979670861568</v>
+      </c>
+      <c r="I3" t="n">
+        <v>2.930300096805421</v>
+      </c>
+      <c r="J3" t="n">
+        <v>2.833494675701839</v>
+      </c>
+      <c r="K3" t="n">
+        <v>6.696030977734753</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>std</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>3.199157789879737</v>
+      </c>
+      <c r="C4" t="n">
+        <v>2.81033967879607</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1.236749789730839</v>
+      </c>
+      <c r="E4" t="n">
+        <v>1.026063280871488</v>
+      </c>
+      <c r="F4" t="n">
+        <v>2.134233371744688</v>
+      </c>
+      <c r="G4" t="n">
+        <v>1.324038759825399</v>
+      </c>
+      <c r="H4" t="n">
+        <v>1.859624914400951</v>
+      </c>
+      <c r="I4" t="n">
+        <v>1.10538744433918</v>
+      </c>
+      <c r="J4" t="n">
+        <v>1.163628831867537</v>
+      </c>
+      <c r="K4" t="n">
+        <v>1.920047673576594</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>min</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>9</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" t="n">
+        <v>2</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" t="n">
+        <v>1</v>
+      </c>
+      <c r="H5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I5" t="n">
+        <v>1</v>
+      </c>
+      <c r="J5" t="n">
+        <v>1</v>
+      </c>
+      <c r="K5" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>25%</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>18</v>
+      </c>
+      <c r="C6" t="n">
+        <v>6</v>
+      </c>
+      <c r="D6" t="n">
+        <v>4</v>
+      </c>
+      <c r="E6" t="n">
+        <v>3</v>
+      </c>
+      <c r="F6" t="n">
+        <v>3</v>
+      </c>
+      <c r="G6" t="n">
+        <v>6</v>
+      </c>
+      <c r="H6" t="n">
+        <v>1</v>
+      </c>
+      <c r="I6" t="n">
+        <v>2</v>
+      </c>
+      <c r="J6" t="n">
+        <v>2</v>
+      </c>
+      <c r="K6" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>50%</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>19</v>
+      </c>
+      <c r="C7" t="n">
+        <v>7</v>
+      </c>
+      <c r="D7" t="n">
+        <v>4</v>
+      </c>
+      <c r="E7" t="n">
+        <v>4</v>
+      </c>
+      <c r="F7" t="n">
+        <v>4</v>
+      </c>
+      <c r="G7" t="n">
+        <v>7</v>
+      </c>
+      <c r="H7" t="n">
+        <v>2</v>
+      </c>
+      <c r="I7" t="n">
+        <v>3</v>
+      </c>
+      <c r="J7" t="n">
+        <v>3</v>
+      </c>
+      <c r="K7" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>75%</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>20</v>
+      </c>
+      <c r="C8" t="n">
+        <v>8</v>
+      </c>
+      <c r="D8" t="n">
+        <v>5</v>
+      </c>
+      <c r="E8" t="n">
+        <v>4</v>
+      </c>
+      <c r="F8" t="n">
+        <v>6</v>
+      </c>
+      <c r="G8" t="n">
+        <v>8</v>
+      </c>
+      <c r="H8" t="n">
+        <v>3</v>
+      </c>
+      <c r="I8" t="n">
+        <v>4</v>
+      </c>
+      <c r="J8" t="n">
+        <v>4</v>
+      </c>
+      <c r="K8" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>max</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>40</v>
+      </c>
+      <c r="C9" t="n">
+        <v>20</v>
+      </c>
+      <c r="D9" t="n">
+        <v>10</v>
+      </c>
+      <c r="E9" t="n">
+        <v>5</v>
+      </c>
+      <c r="F9" t="n">
+        <v>10</v>
+      </c>
+      <c r="G9" t="n">
+        <v>10</v>
+      </c>
+      <c r="H9" t="n">
+        <v>10</v>
+      </c>
+      <c r="I9" t="n">
+        <v>5</v>
+      </c>
+      <c r="J9" t="n">
+        <v>5</v>
+      </c>
+      <c r="K9" t="n">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:X9"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>